<commit_message>
Made changes to QA tools
</commit_message>
<xml_diff>
--- a/docs/assets/downloads/QA log template.xlsx
+++ b/docs/assets/downloads/QA log template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Holly.Goss\github-pages-test\docs\assets\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD53328F-ABDE-45D3-9AE5-79AE3A24518A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAAAD3EC-F32E-4304-8EC6-97AE8E3ECA9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-2145" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="122">
   <si>
     <t>Version 1.2 | May 2024</t>
   </si>
@@ -594,6 +594,12 @@
   </si>
   <si>
     <t>Are calculated totals correct?</t>
+  </si>
+  <si>
+    <t>Further links</t>
+  </si>
+  <si>
+    <t>Ensuring good quality assurance guidance</t>
   </si>
 </sst>
 </file>
@@ -744,7 +750,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -805,6 +811,12 @@
         <bgColor rgb="FFF5F5F5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -1088,7 +1100,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -1327,6 +1339,12 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="31" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1754,10 +1772,10 @@
   <sheetPr>
     <tabColor rgb="FFE2EFDA"/>
   </sheetPr>
-  <dimension ref="A1:BT15"/>
+  <dimension ref="A1:BT17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1889,7 +1907,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:72" s="9" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:72" s="9" customFormat="1" ht="107.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>10</v>
       </c>
@@ -2046,153 +2064,305 @@
       <c r="BS13" s="12"/>
       <c r="BT13" s="12"/>
     </row>
-    <row r="14" spans="1:72" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="13"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
-      <c r="T14" s="2"/>
-      <c r="U14" s="2"/>
-      <c r="V14" s="2"/>
-      <c r="W14" s="2"/>
-      <c r="X14" s="2"/>
-      <c r="Y14" s="2"/>
-      <c r="Z14" s="2"/>
-      <c r="AA14" s="2"/>
-      <c r="AB14" s="2"/>
-      <c r="AC14" s="2"/>
-      <c r="AD14" s="2"/>
-      <c r="AE14" s="2"/>
-      <c r="AF14" s="2"/>
-      <c r="AG14" s="2"/>
-      <c r="AH14" s="2"/>
-      <c r="AI14" s="2"/>
-      <c r="AJ14" s="2"/>
-      <c r="AK14" s="2"/>
-      <c r="AL14" s="2"/>
-      <c r="AM14" s="2"/>
-      <c r="AN14" s="2"/>
-      <c r="AO14" s="2"/>
-      <c r="AP14" s="2"/>
-      <c r="AQ14" s="2"/>
-      <c r="AR14" s="2"/>
-      <c r="AS14" s="2"/>
-      <c r="AT14" s="2"/>
-      <c r="AU14" s="2"/>
-      <c r="AV14" s="2"/>
-      <c r="AW14" s="2"/>
-      <c r="AX14" s="2"/>
-      <c r="AY14" s="2"/>
-      <c r="AZ14" s="2"/>
-      <c r="BA14" s="2"/>
-      <c r="BB14" s="2"/>
-      <c r="BC14" s="2"/>
-      <c r="BD14" s="2"/>
-      <c r="BE14" s="2"/>
-      <c r="BF14" s="2"/>
-      <c r="BG14" s="2"/>
-      <c r="BH14" s="2"/>
-      <c r="BI14" s="2"/>
-      <c r="BJ14" s="2"/>
-      <c r="BK14" s="2"/>
-      <c r="BL14" s="2"/>
-      <c r="BM14" s="2"/>
-      <c r="BN14" s="2"/>
-      <c r="BO14" s="2"/>
-      <c r="BP14" s="2"/>
-      <c r="BQ14" s="2"/>
-      <c r="BR14" s="2"/>
-      <c r="BS14" s="2"/>
-      <c r="BT14" s="2"/>
-    </row>
-    <row r="15" spans="1:72" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="14"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
-      <c r="U15" s="2"/>
-      <c r="V15" s="2"/>
-      <c r="W15" s="2"/>
-      <c r="X15" s="2"/>
-      <c r="Y15" s="2"/>
-      <c r="Z15" s="2"/>
-      <c r="AA15" s="2"/>
-      <c r="AB15" s="2"/>
-      <c r="AC15" s="2"/>
-      <c r="AD15" s="2"/>
-      <c r="AE15" s="2"/>
-      <c r="AF15" s="2"/>
-      <c r="AG15" s="2"/>
-      <c r="AH15" s="2"/>
-      <c r="AI15" s="2"/>
-      <c r="AJ15" s="2"/>
-      <c r="AK15" s="2"/>
-      <c r="AL15" s="2"/>
-      <c r="AM15" s="2"/>
-      <c r="AN15" s="2"/>
-      <c r="AO15" s="2"/>
-      <c r="AP15" s="2"/>
-      <c r="AQ15" s="2"/>
-      <c r="AR15" s="2"/>
-      <c r="AS15" s="2"/>
-      <c r="AT15" s="2"/>
-      <c r="AU15" s="2"/>
-      <c r="AV15" s="2"/>
-      <c r="AW15" s="2"/>
-      <c r="AX15" s="2"/>
-      <c r="AY15" s="2"/>
-      <c r="AZ15" s="2"/>
-      <c r="BA15" s="2"/>
-      <c r="BB15" s="2"/>
-      <c r="BC15" s="2"/>
-      <c r="BD15" s="2"/>
-      <c r="BE15" s="2"/>
-      <c r="BF15" s="2"/>
-      <c r="BG15" s="2"/>
-      <c r="BH15" s="2"/>
-      <c r="BI15" s="2"/>
-      <c r="BJ15" s="2"/>
-      <c r="BK15" s="2"/>
-      <c r="BL15" s="2"/>
-      <c r="BM15" s="2"/>
-      <c r="BN15" s="2"/>
-      <c r="BO15" s="2"/>
-      <c r="BP15" s="2"/>
-      <c r="BQ15" s="2"/>
-      <c r="BR15" s="2"/>
-      <c r="BS15" s="2"/>
-      <c r="BT15" s="2"/>
+    <row r="14" spans="1:72" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="94" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="12"/>
+      <c r="U14" s="12"/>
+      <c r="V14" s="12"/>
+      <c r="W14" s="12"/>
+      <c r="X14" s="12"/>
+      <c r="Y14" s="12"/>
+      <c r="Z14" s="12"/>
+      <c r="AA14" s="12"/>
+      <c r="AB14" s="12"/>
+      <c r="AC14" s="12"/>
+      <c r="AD14" s="12"/>
+      <c r="AE14" s="12"/>
+      <c r="AF14" s="12"/>
+      <c r="AG14" s="12"/>
+      <c r="AH14" s="12"/>
+      <c r="AI14" s="12"/>
+      <c r="AJ14" s="12"/>
+      <c r="AK14" s="12"/>
+      <c r="AL14" s="12"/>
+      <c r="AM14" s="12"/>
+      <c r="AN14" s="12"/>
+      <c r="AO14" s="12"/>
+      <c r="AP14" s="12"/>
+      <c r="AQ14" s="12"/>
+      <c r="AR14" s="12"/>
+      <c r="AS14" s="12"/>
+      <c r="AT14" s="12"/>
+      <c r="AU14" s="12"/>
+      <c r="AV14" s="12"/>
+      <c r="AW14" s="12"/>
+      <c r="AX14" s="12"/>
+      <c r="AY14" s="12"/>
+      <c r="AZ14" s="12"/>
+      <c r="BA14" s="12"/>
+      <c r="BB14" s="12"/>
+      <c r="BC14" s="12"/>
+      <c r="BD14" s="12"/>
+      <c r="BE14" s="12"/>
+      <c r="BF14" s="12"/>
+      <c r="BG14" s="12"/>
+      <c r="BH14" s="12"/>
+      <c r="BI14" s="12"/>
+      <c r="BJ14" s="12"/>
+      <c r="BK14" s="12"/>
+      <c r="BL14" s="12"/>
+      <c r="BM14" s="12"/>
+      <c r="BN14" s="12"/>
+      <c r="BO14" s="12"/>
+      <c r="BP14" s="12"/>
+      <c r="BQ14" s="12"/>
+      <c r="BR14" s="12"/>
+      <c r="BS14" s="12"/>
+      <c r="BT14" s="12"/>
+    </row>
+    <row r="15" spans="1:72" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="95" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="12"/>
+      <c r="X15" s="12"/>
+      <c r="Y15" s="12"/>
+      <c r="Z15" s="12"/>
+      <c r="AA15" s="12"/>
+      <c r="AB15" s="12"/>
+      <c r="AC15" s="12"/>
+      <c r="AD15" s="12"/>
+      <c r="AE15" s="12"/>
+      <c r="AF15" s="12"/>
+      <c r="AG15" s="12"/>
+      <c r="AH15" s="12"/>
+      <c r="AI15" s="12"/>
+      <c r="AJ15" s="12"/>
+      <c r="AK15" s="12"/>
+      <c r="AL15" s="12"/>
+      <c r="AM15" s="12"/>
+      <c r="AN15" s="12"/>
+      <c r="AO15" s="12"/>
+      <c r="AP15" s="12"/>
+      <c r="AQ15" s="12"/>
+      <c r="AR15" s="12"/>
+      <c r="AS15" s="12"/>
+      <c r="AT15" s="12"/>
+      <c r="AU15" s="12"/>
+      <c r="AV15" s="12"/>
+      <c r="AW15" s="12"/>
+      <c r="AX15" s="12"/>
+      <c r="AY15" s="12"/>
+      <c r="AZ15" s="12"/>
+      <c r="BA15" s="12"/>
+      <c r="BB15" s="12"/>
+      <c r="BC15" s="12"/>
+      <c r="BD15" s="12"/>
+      <c r="BE15" s="12"/>
+      <c r="BF15" s="12"/>
+      <c r="BG15" s="12"/>
+      <c r="BH15" s="12"/>
+      <c r="BI15" s="12"/>
+      <c r="BJ15" s="12"/>
+      <c r="BK15" s="12"/>
+      <c r="BL15" s="12"/>
+      <c r="BM15" s="12"/>
+      <c r="BN15" s="12"/>
+      <c r="BO15" s="12"/>
+      <c r="BP15" s="12"/>
+      <c r="BQ15" s="12"/>
+      <c r="BR15" s="12"/>
+      <c r="BS15" s="12"/>
+      <c r="BT15" s="12"/>
+    </row>
+    <row r="16" spans="1:72" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="13"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2"/>
+      <c r="AD16" s="2"/>
+      <c r="AE16" s="2"/>
+      <c r="AF16" s="2"/>
+      <c r="AG16" s="2"/>
+      <c r="AH16" s="2"/>
+      <c r="AI16" s="2"/>
+      <c r="AJ16" s="2"/>
+      <c r="AK16" s="2"/>
+      <c r="AL16" s="2"/>
+      <c r="AM16" s="2"/>
+      <c r="AN16" s="2"/>
+      <c r="AO16" s="2"/>
+      <c r="AP16" s="2"/>
+      <c r="AQ16" s="2"/>
+      <c r="AR16" s="2"/>
+      <c r="AS16" s="2"/>
+      <c r="AT16" s="2"/>
+      <c r="AU16" s="2"/>
+      <c r="AV16" s="2"/>
+      <c r="AW16" s="2"/>
+      <c r="AX16" s="2"/>
+      <c r="AY16" s="2"/>
+      <c r="AZ16" s="2"/>
+      <c r="BA16" s="2"/>
+      <c r="BB16" s="2"/>
+      <c r="BC16" s="2"/>
+      <c r="BD16" s="2"/>
+      <c r="BE16" s="2"/>
+      <c r="BF16" s="2"/>
+      <c r="BG16" s="2"/>
+      <c r="BH16" s="2"/>
+      <c r="BI16" s="2"/>
+      <c r="BJ16" s="2"/>
+      <c r="BK16" s="2"/>
+      <c r="BL16" s="2"/>
+      <c r="BM16" s="2"/>
+      <c r="BN16" s="2"/>
+      <c r="BO16" s="2"/>
+      <c r="BP16" s="2"/>
+      <c r="BQ16" s="2"/>
+      <c r="BR16" s="2"/>
+      <c r="BS16" s="2"/>
+      <c r="BT16" s="2"/>
+    </row>
+    <row r="17" spans="1:72" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="14"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="2"/>
+      <c r="AA17" s="2"/>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="2"/>
+      <c r="AD17" s="2"/>
+      <c r="AE17" s="2"/>
+      <c r="AF17" s="2"/>
+      <c r="AG17" s="2"/>
+      <c r="AH17" s="2"/>
+      <c r="AI17" s="2"/>
+      <c r="AJ17" s="2"/>
+      <c r="AK17" s="2"/>
+      <c r="AL17" s="2"/>
+      <c r="AM17" s="2"/>
+      <c r="AN17" s="2"/>
+      <c r="AO17" s="2"/>
+      <c r="AP17" s="2"/>
+      <c r="AQ17" s="2"/>
+      <c r="AR17" s="2"/>
+      <c r="AS17" s="2"/>
+      <c r="AT17" s="2"/>
+      <c r="AU17" s="2"/>
+      <c r="AV17" s="2"/>
+      <c r="AW17" s="2"/>
+      <c r="AX17" s="2"/>
+      <c r="AY17" s="2"/>
+      <c r="AZ17" s="2"/>
+      <c r="BA17" s="2"/>
+      <c r="BB17" s="2"/>
+      <c r="BC17" s="2"/>
+      <c r="BD17" s="2"/>
+      <c r="BE17" s="2"/>
+      <c r="BF17" s="2"/>
+      <c r="BG17" s="2"/>
+      <c r="BH17" s="2"/>
+      <c r="BI17" s="2"/>
+      <c r="BJ17" s="2"/>
+      <c r="BK17" s="2"/>
+      <c r="BL17" s="2"/>
+      <c r="BM17" s="2"/>
+      <c r="BN17" s="2"/>
+      <c r="BO17" s="2"/>
+      <c r="BP17" s="2"/>
+      <c r="BQ17" s="2"/>
+      <c r="BR17" s="2"/>
+      <c r="BS17" s="2"/>
+      <c r="BT17" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2200,9 +2370,10 @@
     <hyperlink ref="A8" location="'Verification_&amp;_Validation'!A1" display="Verification &amp; Validation" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="A9" location="Reproducibility!A1" display=" Reproducibility" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="A10" location="'Communication_&amp;_outputs'!A1" display="Communication &amp; outputs" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A15" r:id="rId1" tooltip="https://bencuff.github.io/github-pages-test/quality-assurance" xr:uid="{8A1289DD-BA63-44DF-AE62-F7C9F4A383E2}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
-  <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3285,12 +3456,12 @@
       <c r="G1" s="82"/>
     </row>
     <row r="2" spans="1:7" s="70" customFormat="1" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="96" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
     </row>
     <row r="3" spans="1:7" s="38" customFormat="1" ht="48.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="36" t="s">

</xml_diff>